<commit_message>
Renamed domain name to more proper fqdn identifier
</commit_message>
<xml_diff>
--- a/analysis/sherlock/sherlock_datatypes.xlsx
+++ b/analysis/sherlock/sherlock_datatypes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\public\apicrafter\metacrafter-registry\analysis\sherlock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{782C139D-8FD9-413A-91D3-98E898C084E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2A7B1C-66B4-4E90-8322-3F6CB5057F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E45C9A4-0D77-4A3D-B0F3-72D8320F98A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E45C9A4-0D77-4A3D-B0F3-72D8320F98A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="original" sheetId="1" r:id="rId1"/>
+    <sheet name="registry" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="208">
   <si>
     <t>Sherlock Type</t>
   </si>
@@ -617,6 +618,48 @@
   </si>
   <si>
     <t>['May-07', 'May-08', 'May-09', '10-May']</t>
+  </si>
+  <si>
+    <t>Semantic types registry id</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>birthplace</t>
+  </si>
+  <si>
+    <t>orgname</t>
+  </si>
+  <si>
+    <t>uscounty</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>academicdegree</t>
+  </si>
+  <si>
+    <t>isbn10,isbn13</t>
+  </si>
+  <si>
+    <t>person_fullname</t>
+  </si>
+  <si>
+    <t>timerange</t>
+  </si>
+  <si>
+    <t>usstate</t>
   </si>
 </sst>
 </file>
@@ -660,7 +703,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -720,6 +763,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -727,7 +779,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -738,26 +790,14 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -768,32 +808,53 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1112,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F899EA42-C533-43AD-99B9-3ED77C326C2C}">
   <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,31 +1229,31 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1208,7 +1269,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1219,11 +1280,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1272,7 +1333,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1283,25 +1344,25 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
@@ -1310,13 +1371,13 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1332,13 +1393,13 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="6" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1365,18 +1426,18 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
@@ -1385,18 +1446,18 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="2" t="s">
         <v>60</v>
       </c>
@@ -1405,19 +1466,19 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="11" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1425,821 +1486,2307 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="20"/>
+      <c r="B39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="20"/>
+      <c r="B41" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="21"/>
+      <c r="B45" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="5" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="22" t="s">
+      <c r="A47" s="20"/>
+      <c r="B47" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="13" t="s">
+      <c r="A51" s="18"/>
+      <c r="B51" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18" t="s">
+      <c r="A55" s="15"/>
+      <c r="B55" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="18" t="s">
+      <c r="C55" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="13" t="s">
+      <c r="A59" s="15"/>
+      <c r="B59" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C66" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="18" t="s">
+      <c r="A67" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C67" s="18" t="s">
+      <c r="C67" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="13" t="s">
+      <c r="A69" s="15"/>
+      <c r="B69" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-      <c r="B75" s="18" t="s">
+      <c r="A75" s="15"/>
+      <c r="B75" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
-      <c r="B77" s="13" t="s">
+      <c r="A77" s="15"/>
+      <c r="B77" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B79" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="17"/>
-      <c r="B81" s="13" t="s">
+      <c r="A81" s="15"/>
+      <c r="B81" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C81" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
+      <c r="A82" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
-      <c r="B83" s="13" t="s">
+      <c r="A83" s="15"/>
+      <c r="B83" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="C83" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B84" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
-      <c r="B85" s="13" t="s">
+      <c r="A85" s="17"/>
+      <c r="B85" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="13" t="s">
+      <c r="A86" s="18"/>
+      <c r="B86" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
+      <c r="A87" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B88" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
+      <c r="A89" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="16" t="s">
+      <c r="A90" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="21"/>
-      <c r="B91" s="13" t="s">
+      <c r="A91" s="14"/>
+      <c r="B91" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="13" t="s">
+      <c r="A92" s="15"/>
+      <c r="B92" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
+      <c r="A93" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C93" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-      <c r="B94" s="13" t="s">
+      <c r="A94" s="15"/>
+      <c r="B94" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C94" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C95" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C96" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C97" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="13" t="s">
+      <c r="A99" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B99" s="13" t="s">
+      <c r="B99" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C99" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B100" s="13" t="s">
+      <c r="B100" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C100" s="13" t="s">
+      <c r="C100" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C102" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B103" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C103" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+      <c r="A104" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="B104" s="13" t="s">
+      <c r="B104" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="C104" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="17"/>
-      <c r="B105" s="13" t="s">
+      <c r="A105" s="15"/>
+      <c r="B105" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="16" t="s">
+      <c r="A106" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="B106" s="13" t="s">
+      <c r="B106" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="17"/>
-      <c r="B107" s="18" t="s">
+      <c r="A107" s="15"/>
+      <c r="B107" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="C107" s="18" t="s">
+      <c r="C107" s="10" t="s">
         <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A84:A86"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C02B6B-09DB-4C29-95F0-CFFE72FB49DD}">
+  <dimension ref="A1:E107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="15"/>
+      <c r="B69" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D78" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="15"/>
+      <c r="B81" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="15"/>
+      <c r="B83" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D84" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="17"/>
+      <c r="B85" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="18"/>
+      <c r="B86" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D87" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D88" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D89" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="14"/>
+      <c r="B91" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="15"/>
+      <c r="B92" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="15"/>
+      <c r="B94" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D94" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D95" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D96" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D97" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D98" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D99" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D100" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D101" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D102" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D103" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D104" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="15"/>
+      <c r="B105" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D105" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D106" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="15"/>
+      <c r="B107" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D107" s="25" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2268,6 +3815,5 @@
     <mergeCell ref="A28:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>